<commit_message>
Merging Scopus and masterlist
</commit_message>
<xml_diff>
--- a/affs_unique1.xlsx
+++ b/affs_unique1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,11 +552,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>18066</v>
+        <v>18070</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Berkeley</t>
+          <t>University of California _ Berkeley</t>
         </is>
       </c>
     </row>
@@ -572,11 +572,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1892</v>
+        <v>23542</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>University of California _ Los Angeles</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>University of California _ Davis</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>University of California _ San Diego</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Santa Barbara</t>
+          <t>University of California _ Santa Barbara</t>
         </is>
       </c>
     </row>
@@ -1482,51 +1482,51 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>15000</v>
+        <v>15030</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>University Of Massachusetts</t>
+          <t>Centre For Economic Policy Research</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>9545</v>
+        <v>15000</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Federal Reserve Bank Of Chicago</t>
+          <t>University Of Massachusetts</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>9472</v>
+        <v>9545</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Oxford University</t>
+          <t>Federal Reserve Bank Of Chicago</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>9641</v>
+        <v>9472</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>University Of Essex</t>
+          <t>Oxford University</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>9778</v>
+        <v>9641</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Centre For Economic Policy Research</t>
+          <t>University Of Essex</t>
         </is>
       </c>
     </row>
@@ -1552,239 +1552,229 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>21413</v>
+        <v>15518</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Centre for Economic Policy Research </t>
+          <t>Wesleyan University</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>15518</v>
+        <v>21747</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Wesleyan University</t>
+          <t>Brookings Institution</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>21747</v>
+        <v>15903</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Brookings Institution</t>
+          <t>University College London</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>15903</v>
+        <v>10870</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>University College London</t>
+          <t>University Of Texas At Austin</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>10870</v>
+        <v>21949</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>University Of Texas At Austin</t>
+          <t>Universitat Pompeu Fabra</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>21949</v>
+        <v>16066</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Universitat Pompeu Fabra</t>
+          <t>George Washington University</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>16066</v>
+        <v>22100</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>George Washington University</t>
+          <t>The Hebrew University Of Jerusalem</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>22100</v>
+        <v>22136</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>The Hebrew University Of Jerusalem</t>
+          <t>Stockholm University</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>22136</v>
+        <v>22195</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Stockholm University</t>
+          <t>American Bar Foundation</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>22195</v>
+        <v>11205</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>American Bar Foundation</t>
+          <t>Canadian Institute For Advanced Research</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>11205</v>
+        <v>11332</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Canadian Institute For Advanced Research</t>
+          <t>Federal Reserve Board</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>11332</v>
+        <v>22588</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Federal Reserve Board</t>
+          <t>University Of Colorado</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>22588</v>
+        <v>22644</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>University Of Colorado</t>
+          <t>Political Science</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>22644</v>
+        <v>11527</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Political Science</t>
+          <t>Institute For Fiscal Studies</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>11527</v>
+        <v>16907</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Institute For Fiscal Studies</t>
+          <t>Statistics</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>16907</v>
+        <v>11664</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Tulane University</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>11664</v>
+        <v>17030</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Tulane University</t>
+          <t>University Of Oregon</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>17030</v>
+        <v>23163</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>University Of Oregon</t>
+          <t>Arizona State University</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>23163</v>
+        <v>17317</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Arizona State University</t>
+          <t>Uc Berkeley</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>17317</v>
+        <v>17254</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Uc Berkeley</t>
+          <t>University Of Oxford</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>17254</v>
+        <v>17369</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>University Of Oxford</t>
+          <t>Booth School Of Business</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>17369</v>
+        <v>17359</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Booth School Of Business</t>
+          <t>University Of</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>17359</v>
+        <v>17518</v>
       </c>
       <c r="B135" t="inlineStr">
-        <is>
-          <t>University Of</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>17518</v>
-      </c>
-      <c r="B136" t="inlineStr">
         <is>
           <t>Toulouse School Of Economics</t>
         </is>

</xml_diff>